<commit_message>
Added death data to GEMMcoefficients, added GEMM yearly script w heatmap
</commit_message>
<xml_diff>
--- a/GEMMcoefficients.xlsx
+++ b/GEMMcoefficients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrealehatem\Documents\GitHub\ArmeniaPollutionAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA2A2E8-917A-44EE-8B6B-F61BECA20642}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF2BCF7-8547-43EA-95D1-BFFDC5160861}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{98E4048D-D119-4505-BEB0-17765212645F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
   <si>
     <t>NCD+LRI</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>80+</t>
+  </si>
+  <si>
+    <t>Population23</t>
+  </si>
+  <si>
+    <t>Baseline deaths23</t>
+  </si>
+  <si>
+    <t>Death rate</t>
   </si>
 </sst>
 </file>
@@ -439,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588C24D-A40F-4385-8E2F-B12327405D40}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -463,8 +472,17 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -486,8 +504,20 @@
       <c r="G2">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>286+46+47+83+104</f>
+        <v>566</v>
+      </c>
+      <c r="I2">
+        <f>176300+193300+194300+166300+157300</f>
+        <v>887500</v>
+      </c>
+      <c r="J2">
+        <f>H2/I2</f>
+        <v>6.3774647887323947E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -509,8 +539,18 @@
       <c r="G3">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>116</v>
+      </c>
+      <c r="I3">
+        <v>181100</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J14" si="0">H3/I3</f>
+        <v>6.4053009387078966E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -532,8 +572,18 @@
       <c r="G4">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>181</v>
+      </c>
+      <c r="I4">
+        <v>234200</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>7.7284372331340738E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -555,8 +605,18 @@
       <c r="G5">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>242</v>
+      </c>
+      <c r="I5">
+        <v>224800</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1.0765124555160142E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -578,8 +638,18 @@
       <c r="G6">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>347</v>
+      </c>
+      <c r="I6">
+        <v>202600</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1.7127344521224088E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -601,8 +671,18 @@
       <c r="G7">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <v>170400</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>2.9342723004694834E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -624,8 +704,18 @@
       <c r="G8">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>736</v>
+      </c>
+      <c r="I8">
+        <v>163000</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>4.5153374233128834E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -647,8 +737,18 @@
       <c r="G9">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1304</v>
+      </c>
+      <c r="I9">
+        <v>183600</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>7.1023965141612201E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -670,8 +770,18 @@
       <c r="G10">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>2403</v>
+      </c>
+      <c r="I10">
+        <v>229300</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>1.0479720889664196E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -693,8 +803,18 @@
       <c r="G11">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>2952</v>
+      </c>
+      <c r="I11">
+        <v>182500</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>1.6175342465753424E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -716,8 +836,18 @@
       <c r="G12">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>3252</v>
+      </c>
+      <c r="I12">
+        <v>130700</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>2.4881407804131599E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -739,8 +869,18 @@
       <c r="G13">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>2400</v>
+      </c>
+      <c r="I13">
+        <v>57300</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>4.1884816753926704E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -762,8 +902,19 @@
       <c r="G14">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f>3656+5658</f>
+        <v>9314</v>
+      </c>
+      <c r="I14">
+        <v>90700</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.10269018743109151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -786,7 +937,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>

</xml_diff>